<commit_message>
Updated BOM - each unit is $15.73
</commit_message>
<xml_diff>
--- a/accessories/FubarStep/FuabarStep_v10/FubarStep_v10_BOM_SeeedFormat.xlsx
+++ b/accessories/FubarStep/FuabarStep_v10/FubarStep_v10_BOM_SeeedFormat.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\accessories\FubarStep\FuabarStep_v10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="15405" windowHeight="5205" tabRatio="795"/>
   </bookViews>
@@ -561,12 +566,12 @@
     <definedName name="美金對美金" localSheetId="0">#REF!</definedName>
     <definedName name="美金對美金">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>Electronic Engineering BOM List</t>
     <phoneticPr fontId="16" type="noConversion"/>
@@ -900,6 +905,30 @@
   <si>
     <t>FubarStep v1.0 PCB</t>
   </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>Switchcraft</t>
+  </si>
+  <si>
+    <t>RAPC722X</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>68786102LF</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>68016136HLF</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
 </sst>
 </file>
 
@@ -925,18 +954,18 @@
     <numFmt numFmtId="176" formatCode="0%;\(0%\)"/>
     <numFmt numFmtId="177" formatCode="\ \ @"/>
     <numFmt numFmtId="178" formatCode="#,##0_);\(#,##0_)"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="181" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="182" formatCode="_-* #,##0.0\ _k_r_-;\-* #,##0.0\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
-    <numFmt numFmtId="183" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="184" formatCode="&quot;    &quot;@"/>
-    <numFmt numFmtId="185" formatCode="0%_);\(0%\)"/>
-    <numFmt numFmtId="186" formatCode="mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="187" formatCode="_(* #,##0,_);_(* \(#,##0,\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="188" formatCode="\$#,##0.00;\(\$#,##0.00\)"/>
-    <numFmt numFmtId="189" formatCode="\$#,##0;\(\$#,##0\)"/>
-    <numFmt numFmtId="190" formatCode="#,##0;\(#,##0\)"/>
-    <numFmt numFmtId="196" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="180" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.0\ _k_r_-;\-* #,##0.0\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
+    <numFmt numFmtId="182" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="183" formatCode="&quot;    &quot;@"/>
+    <numFmt numFmtId="184" formatCode="0%_);\(0%\)"/>
+    <numFmt numFmtId="185" formatCode="mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="186" formatCode="_(* #,##0,_);_(* \(#,##0,\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="187" formatCode="\$#,##0.00;\(\$#,##0.00\)"/>
+    <numFmt numFmtId="188" formatCode="\$#,##0;\(\$#,##0\)"/>
+    <numFmt numFmtId="189" formatCode="#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="190" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="50">
     <font>
@@ -1178,12 +1207,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1229,9 +1260,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF0057A4"/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1684,19 +1714,19 @@
     <xf numFmtId="174" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="190" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="189" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyAlignment="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="188" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="187" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyProtection="0"/>
-    <xf numFmtId="189" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="188" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
@@ -1719,17 +1749,17 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="183" fontId="24" fillId="4" borderId="0"/>
+    <xf numFmtId="182" fontId="24" fillId="4" borderId="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="174" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="183" fontId="25" fillId="5" borderId="0"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="182" fontId="25" fillId="5" borderId="0"/>
     <xf numFmtId="184" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="186" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -1758,10 +1788,10 @@
     </xf>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="181" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0">
       <protection locked="0"/>
     </xf>
@@ -1819,7 +1849,7 @@
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="348" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1971,8 +2001,6 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="362" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="361" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="361" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="362" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="363" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="360" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1998,31 +2026,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="356" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="362" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="355" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="3" xfId="348" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="3" xfId="348" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="13" borderId="3" xfId="348" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="353" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="360" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="363" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="34" fillId="0" borderId="0" xfId="365" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2041,10 +2049,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="34" fillId="9" borderId="3" xfId="365" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="44" fontId="34" fillId="10" borderId="3" xfId="365" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2061,25 +2065,50 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="0" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="190" fontId="34" fillId="0" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="8" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="34" fillId="8" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="9" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="190" fontId="34" fillId="10" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="190" fontId="34" fillId="10" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="190" fontId="34" fillId="0" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="3" xfId="348" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="10" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="190" fontId="34" fillId="9" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="10" borderId="3" xfId="365" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="3" xfId="348" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="196" fontId="34" fillId="0" borderId="0" xfId="365" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="35" fillId="13" borderId="3" xfId="348" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="34" fillId="9" borderId="3" xfId="365" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="366">
@@ -2456,6 +2485,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -39149,7 +39181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39184,7 +39216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39398,10 +39430,10 @@
   </sheetPr>
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B19" sqref="B19"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="16.5"/>
@@ -39417,9 +39449,9 @@
     <col min="9" max="9" width="33.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="28" style="2" customWidth="1"/>
     <col min="11" max="11" width="22.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="92" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="82" customWidth="1"/>
     <col min="13" max="13" width="26.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="25" style="91" customWidth="1"/>
+    <col min="14" max="14" width="25" style="81" customWidth="1"/>
     <col min="15" max="16384" width="10.28515625" style="4"/>
   </cols>
   <sheetData>
@@ -39428,21 +39460,21 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
-      <c r="N1" s="81"/>
+      <c r="N1" s="72"/>
     </row>
     <row r="2" spans="1:14">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="5"/>
-      <c r="N2" s="82"/>
+      <c r="N2" s="73"/>
     </row>
     <row r="3" spans="1:14" ht="19.5" customHeight="1">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
-      <c r="N3" s="83"/>
+      <c r="N3" s="74"/>
     </row>
     <row r="4" spans="1:14" ht="44.25" customHeight="1">
       <c r="E4" s="1"/>
@@ -39451,7 +39483,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="N4" s="83"/>
+      <c r="N4" s="74"/>
     </row>
     <row r="5" spans="1:14" ht="31.5" customHeight="1">
       <c r="A5" s="11" t="s">
@@ -39464,7 +39496,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="5"/>
-      <c r="N5" s="84"/>
+      <c r="N5" s="75"/>
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A6" s="27" t="s">
@@ -39476,8 +39508,8 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="93"/>
-      <c r="N6" s="85"/>
+      <c r="L6" s="83"/>
+      <c r="N6" s="76"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A7" s="15" t="s">
@@ -39489,8 +39521,8 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="93"/>
-      <c r="N7" s="86"/>
+      <c r="L7" s="83"/>
+      <c r="N7" s="77"/>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A8" s="40" t="s">
@@ -39502,111 +39534,111 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="92"/>
+      <c r="L8" s="82"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="86"/>
+      <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="92"/>
+      <c r="L9" s="82"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="86"/>
+      <c r="N9" s="77"/>
     </row>
     <row r="10" spans="1:14" s="10" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="73" t="s">
+      <c r="J10" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="94" t="s">
+      <c r="L10" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="73" t="s">
+      <c r="M10" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="87" t="s">
+      <c r="N10" s="95" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="87"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="95"/>
     </row>
     <row r="12" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="87"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="95"/>
     </row>
     <row r="13" spans="1:14" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
     </row>
     <row r="14" spans="1:14" s="37" customFormat="1" ht="19.5" customHeight="1">
       <c r="A14" s="28" t="s">
@@ -39621,27 +39653,31 @@
       <c r="D14" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="67" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="68"/>
+      <c r="H14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="66"/>
       <c r="J14" s="29"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="95"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="84">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="M14" s="36"/>
-      <c r="N14" s="88">
-        <f>L14*C14</f>
-        <v>0</v>
+      <c r="N14" s="78">
+        <f t="shared" ref="N14:N30" si="0">L14*C14</f>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="37" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="28">
         <v>2</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="57" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="41">
@@ -39650,27 +39686,31 @@
       <c r="D15" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="52" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="39"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="35"/>
+      <c r="H15" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="I15" s="42"/>
       <c r="J15" s="43"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="95"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="84">
+        <v>0.35</v>
+      </c>
       <c r="M15" s="36"/>
-      <c r="N15" s="88">
-        <f>L15*C15</f>
-        <v>0</v>
+      <c r="N15" s="78">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="37" customFormat="1" ht="19.5" customHeight="1">
       <c r="A16" s="28">
         <v>3</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="57" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="41">
@@ -39679,27 +39719,31 @@
       <c r="D16" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="52" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="35"/>
+      <c r="H16" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="I16" s="45"/>
       <c r="J16" s="43"/>
       <c r="K16" s="46"/>
-      <c r="L16" s="95"/>
+      <c r="L16" s="84">
+        <v>0.12</v>
+      </c>
       <c r="M16" s="36"/>
-      <c r="N16" s="88">
-        <f>L16*C16</f>
-        <v>0</v>
+      <c r="N16" s="78">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="37" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="28">
         <v>4</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="57" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="41">
@@ -39708,27 +39752,31 @@
       <c r="D17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="76" t="s">
+      <c r="E17" s="68" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="35"/>
+      <c r="H17" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="I17" s="42"/>
       <c r="J17" s="43"/>
       <c r="K17" s="44"/>
-      <c r="L17" s="95"/>
+      <c r="L17" s="84">
+        <v>0.15</v>
+      </c>
       <c r="M17" s="36"/>
-      <c r="N17" s="88">
-        <f>L17*C17</f>
-        <v>0</v>
+      <c r="N17" s="78">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="31" customFormat="1" ht="40.5">
+    <row r="18" spans="1:14" s="31" customFormat="1">
       <c r="A18" s="28">
         <v>5</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="57" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="41">
@@ -39737,7 +39785,7 @@
       <c r="D18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="52" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="29"/>
@@ -39745,21 +39793,21 @@
       <c r="H18" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="80" t="s">
+      <c r="I18" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="78" t="s">
+      <c r="J18" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="K18" s="80" t="s">
+      <c r="K18" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="L18" s="96">
+      <c r="L18" s="85">
         <v>4.8500000000000001E-2</v>
       </c>
       <c r="M18" s="30"/>
-      <c r="N18" s="88">
-        <f>L18*C18</f>
+      <c r="N18" s="78">
+        <f t="shared" si="0"/>
         <v>0.58200000000000007</v>
       </c>
     </row>
@@ -39767,7 +39815,7 @@
       <c r="A19" s="28">
         <v>6</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="57" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="41">
@@ -39776,7 +39824,7 @@
       <c r="D19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="52" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="29"/>
@@ -39784,21 +39832,21 @@
       <c r="H19" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="79" t="s">
+      <c r="I19" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="J19" s="78" t="s">
+      <c r="J19" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="K19" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="96">
+      <c r="L19" s="85">
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="M19" s="30"/>
-      <c r="N19" s="88">
-        <f>L19*C19</f>
+      <c r="N19" s="78">
+        <f t="shared" si="0"/>
         <v>0.1704</v>
       </c>
     </row>
@@ -39806,7 +39854,7 @@
       <c r="A20" s="28">
         <v>7</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="57" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="41">
@@ -39815,7 +39863,7 @@
       <c r="D20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="52" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="29"/>
@@ -39823,21 +39871,21 @@
       <c r="H20" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="79" t="s">
+      <c r="I20" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="78" t="s">
+      <c r="J20" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="K20" s="79" t="s">
+      <c r="K20" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="L20" s="96">
+      <c r="L20" s="85">
         <v>0.88990000000000002</v>
       </c>
       <c r="M20" s="30"/>
-      <c r="N20" s="88">
-        <f>L20*C20</f>
+      <c r="N20" s="78">
+        <f t="shared" si="0"/>
         <v>1.7798</v>
       </c>
     </row>
@@ -39845,13 +39893,13 @@
       <c r="A21" s="28">
         <v>8</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="57" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="41">
         <v>2</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="58" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="47" t="s">
@@ -39859,28 +39907,38 @@
       </c>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="96"/>
+      <c r="H21" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="87">
+        <v>13902614</v>
+      </c>
+      <c r="J21" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="87">
+        <v>13902614</v>
+      </c>
+      <c r="L21" s="85">
+        <v>9.2299999999999993E-2</v>
+      </c>
       <c r="M21" s="30"/>
-      <c r="N21" s="88">
-        <f>L21*C21</f>
-        <v>0</v>
+      <c r="N21" s="78">
+        <f t="shared" si="0"/>
+        <v>0.18459999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="31" customFormat="1">
       <c r="A22" s="28">
         <v>9</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="41">
         <v>2</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="58" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="47" t="s">
@@ -39888,115 +39946,149 @@
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="96"/>
+      <c r="H22" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" s="87">
+        <v>393570004</v>
+      </c>
+      <c r="J22" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="87">
+        <v>393570004</v>
+      </c>
+      <c r="L22" s="85">
+        <v>0.56189999999999996</v>
+      </c>
       <c r="M22" s="30"/>
-      <c r="N22" s="88">
-        <f>L22*C22</f>
-        <v>0</v>
+      <c r="N22" s="78">
+        <f t="shared" si="0"/>
+        <v>1.1237999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="31" customFormat="1">
       <c r="A23" s="28">
         <v>10</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="41">
         <v>1</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="52" t="s">
         <v>48</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="96"/>
+      <c r="H23" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="L23" s="85">
+        <v>0.80620000000000003</v>
+      </c>
       <c r="M23" s="30"/>
-      <c r="N23" s="88">
-        <f>L23*C23</f>
-        <v>0</v>
+      <c r="N23" s="78">
+        <f t="shared" si="0"/>
+        <v>0.80620000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="31" customFormat="1">
       <c r="A24" s="28">
         <v>11</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="57" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="41">
         <v>1</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="52" t="s">
         <v>50</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="I24" s="45"/>
       <c r="J24" s="43"/>
       <c r="K24" s="46"/>
-      <c r="L24" s="96"/>
+      <c r="L24" s="85">
+        <v>0.03</v>
+      </c>
       <c r="M24" s="30"/>
-      <c r="N24" s="88">
-        <f>L24*C24</f>
-        <v>0</v>
+      <c r="N24" s="78">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="31" customFormat="1">
       <c r="A25" s="28">
         <v>12</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="57" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="41">
         <v>1</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="52" t="s">
         <v>52</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="96"/>
+      <c r="H25" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="87">
+        <v>393570002</v>
+      </c>
+      <c r="J25" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" s="87">
+        <v>393570002</v>
+      </c>
+      <c r="L25" s="85">
+        <v>0.27210000000000001</v>
+      </c>
       <c r="M25" s="30"/>
-      <c r="N25" s="88">
-        <f>L25*C25</f>
-        <v>0</v>
+      <c r="N25" s="78">
+        <f t="shared" si="0"/>
+        <v>0.27210000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="31" customFormat="1">
       <c r="A26" s="28">
         <v>13</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="41">
         <v>1</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="58" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="47" t="s">
@@ -40004,28 +40096,38 @@
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="96"/>
+      <c r="H26" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="85">
+        <v>0.39419999999999999</v>
+      </c>
       <c r="M26" s="30"/>
-      <c r="N26" s="88">
-        <f>L26*C26</f>
-        <v>0</v>
+      <c r="N26" s="78">
+        <f t="shared" si="0"/>
+        <v>0.39419999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="31" customFormat="1">
       <c r="A27" s="28">
         <v>14</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="57" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="41">
         <v>1</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="58" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="47" t="s">
@@ -40039,18 +40141,18 @@
       <c r="I27" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="J27" s="78" t="s">
+      <c r="J27" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="77" t="s">
+      <c r="K27" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="L27" s="96">
+      <c r="L27" s="85">
         <v>4.3</v>
       </c>
       <c r="M27" s="30"/>
-      <c r="N27" s="88">
-        <f>L27*C27</f>
+      <c r="N27" s="78">
+        <f t="shared" si="0"/>
         <v>4.3</v>
       </c>
     </row>
@@ -40058,42 +40160,52 @@
       <c r="A28" s="28">
         <v>15</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="57" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="41">
         <v>1</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="52" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="96"/>
+      <c r="H28" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="L28" s="85">
+        <v>7.2599999999999998E-2</v>
+      </c>
       <c r="M28" s="30"/>
-      <c r="N28" s="88">
-        <f>L28*C28</f>
-        <v>0</v>
+      <c r="N28" s="78">
+        <f t="shared" si="0"/>
+        <v>7.2599999999999998E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="31" customFormat="1">
       <c r="A29" s="28">
         <v>16</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="57" t="s">
         <v>71</v>
       </c>
       <c r="C29" s="41">
         <v>1</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="58" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="47" t="s">
@@ -40107,20 +40219,20 @@
       <c r="I29" s="48"/>
       <c r="J29" s="43"/>
       <c r="K29" s="49"/>
-      <c r="L29" s="96">
+      <c r="L29" s="85">
         <v>3.4</v>
       </c>
       <c r="M29" s="30"/>
-      <c r="N29" s="88">
-        <f>L29*C29</f>
+      <c r="N29" s="78">
+        <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="31" customFormat="1">
       <c r="A30" s="28"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="60"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="58"/>
       <c r="E30" s="35"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
@@ -40128,18 +40240,18 @@
       <c r="I30" s="35"/>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="96"/>
+      <c r="L30" s="85"/>
       <c r="M30" s="30"/>
-      <c r="N30" s="88">
-        <f>L30*C30</f>
+      <c r="N30" s="78">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="31" customFormat="1">
       <c r="A31" s="28"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="91"/>
       <c r="E31" s="35"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
@@ -40147,52 +40259,52 @@
       <c r="I31" s="35"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="96"/>
+      <c r="L31" s="85"/>
       <c r="M31" s="30"/>
-      <c r="N31" s="89"/>
+      <c r="N31" s="79"/>
     </row>
     <row r="32" spans="1:14" s="31" customFormat="1">
       <c r="A32" s="28"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="55"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="35"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="96"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="85"/>
       <c r="M32" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N32" s="89">
+      <c r="N32" s="79">
         <f>SUM(N14:N31)</f>
-        <v>10.232200000000001</v>
+        <v>15.7257</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="31" customFormat="1">
       <c r="A33" s="28"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="57"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="35"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="96"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="85"/>
       <c r="M33" s="30"/>
-      <c r="N33" s="89"/>
+      <c r="N33" s="79"/>
     </row>
     <row r="34" spans="1:14" s="31" customFormat="1">
       <c r="A34" s="28"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="60"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="58"/>
       <c r="E34" s="35"/>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
@@ -40200,31 +40312,31 @@
       <c r="I34" s="35"/>
       <c r="J34" s="29"/>
       <c r="K34" s="29"/>
-      <c r="L34" s="96"/>
+      <c r="L34" s="85"/>
       <c r="M34" s="30"/>
-      <c r="N34" s="89"/>
+      <c r="N34" s="79"/>
     </row>
     <row r="35" spans="1:14" s="31" customFormat="1">
       <c r="A35" s="28"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="65"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="63"/>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
       <c r="H35" s="35"/>
       <c r="I35" s="35"/>
       <c r="J35" s="29"/>
       <c r="K35" s="32"/>
-      <c r="L35" s="96"/>
+      <c r="L35" s="85"/>
       <c r="M35" s="30"/>
-      <c r="N35" s="89"/>
+      <c r="N35" s="79"/>
     </row>
     <row r="36" spans="1:14" s="31" customFormat="1">
       <c r="A36" s="28"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="60"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="58"/>
       <c r="E36" s="35"/>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -40232,9 +40344,9 @@
       <c r="I36" s="35"/>
       <c r="J36" s="29"/>
       <c r="K36" s="32"/>
-      <c r="L36" s="96"/>
+      <c r="L36" s="85"/>
       <c r="M36" s="30"/>
-      <c r="N36" s="89"/>
+      <c r="N36" s="79"/>
     </row>
     <row r="37" spans="1:14" s="31" customFormat="1">
       <c r="A37" s="28"/>
@@ -40248,9 +40360,9 @@
       <c r="I37" s="35"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
-      <c r="L37" s="96"/>
+      <c r="L37" s="85"/>
       <c r="M37" s="30"/>
-      <c r="N37" s="89"/>
+      <c r="N37" s="79"/>
     </row>
     <row r="38" spans="1:14" s="31" customFormat="1">
       <c r="A38" s="28"/>
@@ -40264,9 +40376,9 @@
       <c r="I38" s="35"/>
       <c r="J38" s="33"/>
       <c r="K38" s="33"/>
-      <c r="L38" s="96"/>
+      <c r="L38" s="85"/>
       <c r="M38" s="30"/>
-      <c r="N38" s="89"/>
+      <c r="N38" s="79"/>
     </row>
     <row r="39" spans="1:14" s="31" customFormat="1">
       <c r="A39" s="28"/>
@@ -40280,9 +40392,9 @@
       <c r="I39" s="35"/>
       <c r="J39" s="29"/>
       <c r="K39" s="29"/>
-      <c r="L39" s="96"/>
+      <c r="L39" s="85"/>
       <c r="M39" s="30"/>
-      <c r="N39" s="89"/>
+      <c r="N39" s="79"/>
     </row>
     <row r="40" spans="1:14" s="31" customFormat="1">
       <c r="A40" s="28"/>
@@ -40296,9 +40408,9 @@
       <c r="I40" s="35"/>
       <c r="J40" s="29"/>
       <c r="K40" s="29"/>
-      <c r="L40" s="96"/>
+      <c r="L40" s="85"/>
       <c r="M40" s="30"/>
-      <c r="N40" s="89"/>
+      <c r="N40" s="79"/>
     </row>
     <row r="41" spans="1:14" s="31" customFormat="1">
       <c r="A41" s="28"/>
@@ -40312,9 +40424,9 @@
       <c r="I41" s="35"/>
       <c r="J41" s="33"/>
       <c r="K41" s="33"/>
-      <c r="L41" s="96"/>
+      <c r="L41" s="85"/>
       <c r="M41" s="30"/>
-      <c r="N41" s="89"/>
+      <c r="N41" s="79"/>
     </row>
     <row r="42" spans="1:14" s="31" customFormat="1">
       <c r="A42" s="28"/>
@@ -40328,9 +40440,9 @@
       <c r="I42" s="35"/>
       <c r="J42" s="29"/>
       <c r="K42" s="29"/>
-      <c r="L42" s="96"/>
+      <c r="L42" s="85"/>
       <c r="M42" s="30"/>
-      <c r="N42" s="89"/>
+      <c r="N42" s="79"/>
     </row>
     <row r="43" spans="1:14" s="31" customFormat="1">
       <c r="A43" s="28"/>
@@ -40344,9 +40456,9 @@
       <c r="I43" s="35"/>
       <c r="J43" s="33"/>
       <c r="K43" s="33"/>
-      <c r="L43" s="96"/>
+      <c r="L43" s="85"/>
       <c r="M43" s="30"/>
-      <c r="N43" s="89"/>
+      <c r="N43" s="79"/>
     </row>
     <row r="44" spans="1:14" s="31" customFormat="1">
       <c r="A44" s="28"/>
@@ -40360,9 +40472,9 @@
       <c r="I44" s="35"/>
       <c r="J44" s="33"/>
       <c r="K44" s="33"/>
-      <c r="L44" s="96"/>
+      <c r="L44" s="85"/>
       <c r="M44" s="30"/>
-      <c r="N44" s="89"/>
+      <c r="N44" s="79"/>
     </row>
     <row r="45" spans="1:14" s="31" customFormat="1">
       <c r="A45" s="28"/>
@@ -40376,9 +40488,9 @@
       <c r="I45" s="35"/>
       <c r="J45" s="29"/>
       <c r="K45" s="29"/>
-      <c r="L45" s="96"/>
+      <c r="L45" s="85"/>
       <c r="M45" s="30"/>
-      <c r="N45" s="89"/>
+      <c r="N45" s="79"/>
     </row>
     <row r="46" spans="1:14" s="31" customFormat="1">
       <c r="A46" s="28"/>
@@ -40392,9 +40504,9 @@
       <c r="I46" s="35"/>
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
-      <c r="L46" s="96"/>
+      <c r="L46" s="85"/>
       <c r="M46" s="30"/>
-      <c r="N46" s="89"/>
+      <c r="N46" s="79"/>
     </row>
     <row r="47" spans="1:14" s="31" customFormat="1">
       <c r="A47" s="28"/>
@@ -40408,9 +40520,9 @@
       <c r="I47" s="35"/>
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
-      <c r="L47" s="96"/>
+      <c r="L47" s="85"/>
       <c r="M47" s="30"/>
-      <c r="N47" s="89"/>
+      <c r="N47" s="79"/>
     </row>
     <row r="48" spans="1:14" s="31" customFormat="1">
       <c r="A48" s="28"/>
@@ -40424,9 +40536,9 @@
       <c r="I48" s="35"/>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
-      <c r="L48" s="96"/>
+      <c r="L48" s="85"/>
       <c r="M48" s="30"/>
-      <c r="N48" s="89"/>
+      <c r="N48" s="79"/>
     </row>
     <row r="49" spans="1:14" s="31" customFormat="1">
       <c r="A49" s="28"/>
@@ -40440,9 +40552,9 @@
       <c r="I49" s="35"/>
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
-      <c r="L49" s="96"/>
+      <c r="L49" s="85"/>
       <c r="M49" s="30"/>
-      <c r="N49" s="89"/>
+      <c r="N49" s="79"/>
     </row>
     <row r="50" spans="1:14" s="31" customFormat="1">
       <c r="A50" s="28"/>
@@ -40456,9 +40568,9 @@
       <c r="I50" s="38"/>
       <c r="J50" s="29"/>
       <c r="K50" s="29"/>
-      <c r="L50" s="96"/>
+      <c r="L50" s="85"/>
       <c r="M50" s="30"/>
-      <c r="N50" s="89"/>
+      <c r="N50" s="79"/>
     </row>
     <row r="51" spans="1:14" s="31" customFormat="1" ht="17.25" customHeight="1">
       <c r="A51" s="28"/>
@@ -40472,9 +40584,9 @@
       <c r="I51" s="38"/>
       <c r="J51" s="29"/>
       <c r="K51" s="29"/>
-      <c r="L51" s="96"/>
+      <c r="L51" s="85"/>
       <c r="M51" s="30"/>
-      <c r="N51" s="89"/>
+      <c r="N51" s="79"/>
     </row>
     <row r="52" spans="1:14" s="31" customFormat="1">
       <c r="A52" s="28"/>
@@ -40488,9 +40600,9 @@
       <c r="I52" s="35"/>
       <c r="J52" s="29"/>
       <c r="K52" s="29"/>
-      <c r="L52" s="96"/>
+      <c r="L52" s="85"/>
       <c r="M52" s="30"/>
-      <c r="N52" s="89"/>
+      <c r="N52" s="79"/>
     </row>
     <row r="53" spans="1:14" s="31" customFormat="1">
       <c r="A53" s="28"/>
@@ -40504,9 +40616,9 @@
       <c r="I53" s="35"/>
       <c r="J53" s="29"/>
       <c r="K53" s="29"/>
-      <c r="L53" s="96"/>
+      <c r="L53" s="85"/>
       <c r="M53" s="30"/>
-      <c r="N53" s="89"/>
+      <c r="N53" s="79"/>
     </row>
     <row r="54" spans="1:14" s="31" customFormat="1">
       <c r="A54" s="28"/>
@@ -40520,9 +40632,9 @@
       <c r="I54" s="35"/>
       <c r="J54" s="29"/>
       <c r="K54" s="29"/>
-      <c r="L54" s="96"/>
+      <c r="L54" s="85"/>
       <c r="M54" s="30"/>
-      <c r="N54" s="89"/>
+      <c r="N54" s="79"/>
     </row>
     <row r="55" spans="1:14" s="31" customFormat="1">
       <c r="A55" s="28"/>
@@ -40536,9 +40648,9 @@
       <c r="I55" s="35"/>
       <c r="J55" s="29"/>
       <c r="K55" s="29"/>
-      <c r="L55" s="96"/>
+      <c r="L55" s="85"/>
       <c r="M55" s="30"/>
-      <c r="N55" s="89"/>
+      <c r="N55" s="79"/>
     </row>
     <row r="56" spans="1:14" s="31" customFormat="1">
       <c r="A56" s="28"/>
@@ -40552,9 +40664,9 @@
       <c r="I56" s="35"/>
       <c r="J56" s="29"/>
       <c r="K56" s="29"/>
-      <c r="L56" s="96"/>
+      <c r="L56" s="85"/>
       <c r="M56" s="30"/>
-      <c r="N56" s="89"/>
+      <c r="N56" s="79"/>
     </row>
     <row r="57" spans="1:14" s="31" customFormat="1">
       <c r="A57" s="28"/>
@@ -40568,9 +40680,9 @@
       <c r="I57" s="35"/>
       <c r="J57" s="29"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="96"/>
+      <c r="L57" s="85"/>
       <c r="M57" s="30"/>
-      <c r="N57" s="89"/>
+      <c r="N57" s="79"/>
     </row>
     <row r="58" spans="1:14" s="31" customFormat="1">
       <c r="A58" s="28"/>
@@ -40584,9 +40696,9 @@
       <c r="I58" s="38"/>
       <c r="J58" s="29"/>
       <c r="K58" s="29"/>
-      <c r="L58" s="96"/>
+      <c r="L58" s="85"/>
       <c r="M58" s="30"/>
-      <c r="N58" s="89"/>
+      <c r="N58" s="79"/>
     </row>
     <row r="59" spans="1:14" s="31" customFormat="1">
       <c r="A59" s="28"/>
@@ -40600,9 +40712,9 @@
       <c r="I59" s="35"/>
       <c r="J59" s="29"/>
       <c r="K59" s="29"/>
-      <c r="L59" s="96"/>
+      <c r="L59" s="85"/>
       <c r="M59" s="30"/>
-      <c r="N59" s="89"/>
+      <c r="N59" s="79"/>
     </row>
     <row r="60" spans="1:14" s="31" customFormat="1">
       <c r="A60" s="28"/>
@@ -40616,9 +40728,9 @@
       <c r="I60" s="35"/>
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
-      <c r="L60" s="96"/>
+      <c r="L60" s="85"/>
       <c r="M60" s="30"/>
-      <c r="N60" s="89"/>
+      <c r="N60" s="79"/>
     </row>
     <row r="61" spans="1:14" s="31" customFormat="1">
       <c r="A61" s="28"/>
@@ -40632,9 +40744,9 @@
       <c r="I61" s="35"/>
       <c r="J61" s="29"/>
       <c r="K61" s="29"/>
-      <c r="L61" s="96"/>
+      <c r="L61" s="85"/>
       <c r="M61" s="30"/>
-      <c r="N61" s="89"/>
+      <c r="N61" s="79"/>
     </row>
     <row r="62" spans="1:14" s="31" customFormat="1">
       <c r="A62" s="28"/>
@@ -40648,9 +40760,9 @@
       <c r="I62" s="35"/>
       <c r="J62" s="29"/>
       <c r="K62" s="29"/>
-      <c r="L62" s="96"/>
+      <c r="L62" s="85"/>
       <c r="M62" s="30"/>
-      <c r="N62" s="89"/>
+      <c r="N62" s="79"/>
     </row>
     <row r="63" spans="1:14" s="31" customFormat="1">
       <c r="A63" s="28"/>
@@ -40664,9 +40776,9 @@
       <c r="I63" s="35"/>
       <c r="J63" s="29"/>
       <c r="K63" s="29"/>
-      <c r="L63" s="96"/>
+      <c r="L63" s="85"/>
       <c r="M63" s="30"/>
-      <c r="N63" s="89"/>
+      <c r="N63" s="79"/>
     </row>
     <row r="64" spans="1:14" s="31" customFormat="1">
       <c r="A64" s="28"/>
@@ -40680,9 +40792,9 @@
       <c r="I64" s="35"/>
       <c r="J64" s="29"/>
       <c r="K64" s="29"/>
-      <c r="L64" s="96"/>
+      <c r="L64" s="85"/>
       <c r="M64" s="30"/>
-      <c r="N64" s="89"/>
+      <c r="N64" s="79"/>
     </row>
     <row r="65" spans="1:14" s="31" customFormat="1">
       <c r="A65" s="28"/>
@@ -40696,9 +40808,9 @@
       <c r="I65" s="35"/>
       <c r="J65" s="29"/>
       <c r="K65" s="29"/>
-      <c r="L65" s="96"/>
+      <c r="L65" s="85"/>
       <c r="M65" s="30"/>
-      <c r="N65" s="89"/>
+      <c r="N65" s="79"/>
     </row>
     <row r="66" spans="1:14" s="31" customFormat="1">
       <c r="A66" s="28"/>
@@ -40712,9 +40824,9 @@
       <c r="I66" s="35"/>
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
-      <c r="L66" s="96"/>
+      <c r="L66" s="85"/>
       <c r="M66" s="30"/>
-      <c r="N66" s="89"/>
+      <c r="N66" s="79"/>
     </row>
     <row r="67" spans="1:14" s="31" customFormat="1">
       <c r="A67" s="28"/>
@@ -40728,9 +40840,9 @@
       <c r="I67" s="35"/>
       <c r="J67" s="29"/>
       <c r="K67" s="29"/>
-      <c r="L67" s="96"/>
+      <c r="L67" s="85"/>
       <c r="M67" s="30"/>
-      <c r="N67" s="89"/>
+      <c r="N67" s="79"/>
     </row>
     <row r="68" spans="1:14" s="31" customFormat="1">
       <c r="A68" s="28"/>
@@ -40744,9 +40856,9 @@
       <c r="I68" s="35"/>
       <c r="J68" s="29"/>
       <c r="K68" s="29"/>
-      <c r="L68" s="96"/>
+      <c r="L68" s="85"/>
       <c r="M68" s="30"/>
-      <c r="N68" s="89"/>
+      <c r="N68" s="79"/>
     </row>
     <row r="69" spans="1:14" s="31" customFormat="1">
       <c r="A69" s="28"/>
@@ -40760,9 +40872,9 @@
       <c r="I69" s="35"/>
       <c r="J69" s="29"/>
       <c r="K69" s="29"/>
-      <c r="L69" s="96"/>
+      <c r="L69" s="85"/>
       <c r="M69" s="30"/>
-      <c r="N69" s="89"/>
+      <c r="N69" s="79"/>
     </row>
     <row r="70" spans="1:14" s="31" customFormat="1">
       <c r="A70" s="28"/>
@@ -40776,9 +40888,9 @@
       <c r="I70" s="35"/>
       <c r="J70" s="29"/>
       <c r="K70" s="29"/>
-      <c r="L70" s="96"/>
+      <c r="L70" s="85"/>
       <c r="M70" s="30"/>
-      <c r="N70" s="89"/>
+      <c r="N70" s="79"/>
     </row>
     <row r="71" spans="1:14" s="31" customFormat="1">
       <c r="A71" s="28"/>
@@ -40792,9 +40904,9 @@
       <c r="I71" s="35"/>
       <c r="J71" s="33"/>
       <c r="K71" s="33"/>
-      <c r="L71" s="96"/>
+      <c r="L71" s="85"/>
       <c r="M71" s="30"/>
-      <c r="N71" s="89"/>
+      <c r="N71" s="79"/>
     </row>
     <row r="72" spans="1:14" s="31" customFormat="1">
       <c r="A72" s="28"/>
@@ -40808,9 +40920,9 @@
       <c r="I72" s="35"/>
       <c r="J72" s="29"/>
       <c r="K72" s="29"/>
-      <c r="L72" s="96"/>
+      <c r="L72" s="85"/>
       <c r="M72" s="30"/>
-      <c r="N72" s="89"/>
+      <c r="N72" s="79"/>
     </row>
     <row r="73" spans="1:14" s="31" customFormat="1">
       <c r="A73" s="28"/>
@@ -40824,9 +40936,9 @@
       <c r="I73" s="35"/>
       <c r="J73" s="29"/>
       <c r="K73" s="29"/>
-      <c r="L73" s="96"/>
+      <c r="L73" s="85"/>
       <c r="M73" s="30"/>
-      <c r="N73" s="89"/>
+      <c r="N73" s="79"/>
     </row>
     <row r="74" spans="1:14" s="26" customFormat="1">
       <c r="A74" s="23"/>
@@ -40840,9 +40952,9 @@
       <c r="I74" s="8"/>
       <c r="J74" s="24"/>
       <c r="K74" s="24"/>
-      <c r="L74" s="97"/>
+      <c r="L74" s="86"/>
       <c r="M74" s="25"/>
-      <c r="N74" s="90"/>
+      <c r="N74" s="80"/>
     </row>
     <row r="75" spans="1:14" ht="24" customHeight="1">
       <c r="A75" s="22" t="s">

</xml_diff>